<commit_message>
Add Gemini 2.0 Models
</commit_message>
<xml_diff>
--- a/Scores.xlsx
+++ b/Scores.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>نام مدل</t>
   </si>
@@ -80,6 +80,15 @@
   </si>
   <si>
     <t>امتیاز (10)</t>
+  </si>
+  <si>
+    <t>gemini-2.0-flash</t>
+  </si>
+  <si>
+    <t>gemini-2.0-pro-exp-02-05</t>
+  </si>
+  <si>
+    <t>gemini-2.0-flash-exp</t>
   </si>
 </sst>
 </file>
@@ -466,7 +475,7 @@
   <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
@@ -644,13 +653,28 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="2"/>
+      <c r="A22" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="2"/>
+      <c r="A23" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="2"/>
+      <c r="A24" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="2"/>

</xml_diff>